<commit_message>
Updated fields in .xlsx to allow for reporting characteristics and calibration fit scores
</commit_message>
<xml_diff>
--- a/project/cascade_belarus.xlsx
+++ b/project/cascade_belarus.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
@@ -14,8 +19,11 @@
     <sheet name="Parameters" sheetId="3" r:id="rId5"/>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="552">
   <si>
     <t>Code Label</t>
   </si>
@@ -1419,24 +1427,6 @@
   </si>
   <si>
     <t>num_xddis</t>
-  </si>
-  <si>
-    <t>Number of SN DS-TB related deaths</t>
-  </si>
-  <si>
-    <t>Number of SN MDR TB-related deaths</t>
-  </si>
-  <si>
-    <t>Number of SN XDR TB-related deaths</t>
-  </si>
-  <si>
-    <t>Number of SP DS-TB related deaths</t>
-  </si>
-  <si>
-    <t>Number of SP MDR TB-related deaths</t>
-  </si>
-  <si>
-    <t>Number of SP XDR TB-related deaths</t>
   </si>
   <si>
     <t>Number of Total DS-TB related deaths</t>
@@ -1868,6 +1858,24 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>Percentage of SN DS-TB related deaths</t>
+  </si>
+  <si>
+    <t>Percentage of SN MDR TB-related deaths</t>
+  </si>
+  <si>
+    <t>Percentage of SN XDR TB-related deaths</t>
+  </si>
+  <si>
+    <t>Percentage of SP DS-TB related deaths</t>
+  </si>
+  <si>
+    <t>Percentage of SP MDR TB-related deaths</t>
+  </si>
+  <si>
+    <t>Percentage of SP XDR TB-related deaths</t>
   </si>
 </sst>
 </file>
@@ -2984,23 +2992,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>338</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3012,17 +3015,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="8.77734375" style="2"/>
+    <col min="4" max="4" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3056,7 +3059,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3067,7 +3070,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>275</v>
       </c>
@@ -3078,7 +3081,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>276</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>277</v>
       </c>
@@ -3100,7 +3103,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>278</v>
       </c>
@@ -3111,7 +3114,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>272</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>273</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>194</v>
       </c>
@@ -3183,7 +3186,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>195</v>
       </c>
@@ -3194,7 +3197,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -3205,7 +3208,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>197</v>
       </c>
@@ -3216,7 +3219,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>199</v>
       </c>
@@ -3238,7 +3241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>200</v>
       </c>
@@ -3249,7 +3252,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>201</v>
       </c>
@@ -3260,7 +3263,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>202</v>
       </c>
@@ -3271,7 +3274,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>274</v>
       </c>
@@ -3285,7 +3288,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>203</v>
       </c>
@@ -3296,7 +3299,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>204</v>
       </c>
@@ -3307,7 +3310,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -3318,7 +3321,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>206</v>
       </c>
@@ -3329,7 +3332,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -3340,7 +3343,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>208</v>
       </c>
@@ -3351,7 +3354,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>209</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>210</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>211</v>
       </c>
@@ -3384,7 +3387,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>132</v>
       </c>
@@ -3395,7 +3398,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -3412,7 +3415,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>339</v>
       </c>
@@ -3442,11 +3445,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3458,14 +3456,14 @@
       <selection activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="11" width="5.33203125" customWidth="1"/>
     <col min="12" max="12" width="5.33203125" style="2" customWidth="1"/>
     <col min="13" max="35" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>339</v>
@@ -3570,7 +3568,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>339</v>
       </c>
@@ -3613,7 +3611,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3658,7 +3656,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3701,7 +3699,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>275</v>
       </c>
@@ -3748,7 +3746,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>276</v>
       </c>
@@ -3795,7 +3793,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>277</v>
       </c>
@@ -3840,7 +3838,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>278</v>
       </c>
@@ -3885,7 +3883,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>279</v>
       </c>
@@ -3930,7 +3928,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>280</v>
       </c>
@@ -3975,7 +3973,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -4018,7 +4016,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>272</v>
       </c>
@@ -4061,7 +4059,7 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="22"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>273</v>
       </c>
@@ -4106,7 +4104,7 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="11"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>194</v>
       </c>
@@ -4147,13 +4145,13 @@
         <v>353</v>
       </c>
       <c r="AH14" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AI14" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>195</v>
       </c>
@@ -4194,13 +4192,13 @@
         <v>353</v>
       </c>
       <c r="AH15" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AI15" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>196</v>
       </c>
@@ -4249,7 +4247,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>197</v>
       </c>
@@ -4290,13 +4288,13 @@
         <v>354</v>
       </c>
       <c r="AH17" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AI17" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>198</v>
       </c>
@@ -4337,13 +4335,13 @@
         <v>354</v>
       </c>
       <c r="AH18" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AI18" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>199</v>
       </c>
@@ -4392,7 +4390,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>200</v>
       </c>
@@ -4433,13 +4431,13 @@
         <v>355</v>
       </c>
       <c r="AH20" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AI20" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>201</v>
       </c>
@@ -4480,13 +4478,13 @@
         <v>355</v>
       </c>
       <c r="AH21" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AI21" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>202</v>
       </c>
@@ -4533,7 +4531,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>274</v>
       </c>
@@ -4578,7 +4576,7 @@
       <c r="AH23" s="7"/>
       <c r="AI23" s="8"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>203</v>
       </c>
@@ -4619,13 +4617,13 @@
         <v>432</v>
       </c>
       <c r="AH24" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AI24" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>204</v>
       </c>
@@ -4666,13 +4664,13 @@
         <v>432</v>
       </c>
       <c r="AH25" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AI25" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>205</v>
       </c>
@@ -4721,7 +4719,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>206</v>
       </c>
@@ -4762,13 +4760,13 @@
         <v>356</v>
       </c>
       <c r="AH27" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AI27" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>207</v>
       </c>
@@ -4809,13 +4807,13 @@
         <v>356</v>
       </c>
       <c r="AH28" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AI28" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>208</v>
       </c>
@@ -4864,7 +4862,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>209</v>
       </c>
@@ -4905,13 +4903,13 @@
         <v>357</v>
       </c>
       <c r="AH30" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AI30" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>210</v>
       </c>
@@ -4952,13 +4950,13 @@
         <v>357</v>
       </c>
       <c r="AH31" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AI31" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>211</v>
       </c>
@@ -5005,7 +5003,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>132</v>
       </c>
@@ -5048,7 +5046,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>87</v>
       </c>
@@ -5087,7 +5085,7 @@
       <c r="AH34" s="10"/>
       <c r="AI34" s="11"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>88</v>
       </c>
@@ -5129,11 +5127,6 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5141,36 +5134,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="16" width="8.77734375" customWidth="1"/>
+    <col min="12" max="16" width="8.83203125" customWidth="1"/>
     <col min="17" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5187,7 +5180,7 @@
         <v>57</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>103</v>
@@ -5202,7 +5195,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -5231,7 +5224,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -5239,13 +5232,13 @@
         <v>141</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J3" t="s">
         <v>194</v>
@@ -5254,7 +5247,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -5262,13 +5255,13 @@
         <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J4" t="s">
         <v>197</v>
@@ -5277,7 +5270,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -5285,13 +5278,13 @@
         <v>143</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D5" s="2">
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J5" t="s">
         <v>200</v>
@@ -5300,7 +5293,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>241</v>
       </c>
@@ -5308,13 +5301,13 @@
         <v>164</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D6" s="2">
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J6" t="s">
         <v>203</v>
@@ -5323,7 +5316,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>242</v>
       </c>
@@ -5331,13 +5324,13 @@
         <v>165</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D7" s="2">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J7" t="s">
         <v>206</v>
@@ -5346,7 +5339,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>243</v>
       </c>
@@ -5354,13 +5347,13 @@
         <v>166</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D8" s="2">
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J8" t="s">
         <v>209</v>
@@ -5369,7 +5362,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>215</v>
       </c>
@@ -5377,13 +5370,13 @@
         <v>188</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J9" t="s">
         <v>273</v>
@@ -5407,7 +5400,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -5415,13 +5408,13 @@
         <v>190</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D10" s="2">
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J10" t="s">
         <v>274</v>
@@ -5445,15 +5438,15 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -5468,7 +5461,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -5506,7 +5499,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -5514,7 +5507,7 @@
         <v>108</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>93</v>
@@ -5529,7 +5522,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>216</v>
       </c>
@@ -5543,7 +5536,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>93</v>
@@ -5555,7 +5548,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>217</v>
       </c>
@@ -5569,7 +5562,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>93</v>
@@ -5581,7 +5574,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>218</v>
       </c>
@@ -5595,7 +5588,7 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>93</v>
@@ -5607,7 +5600,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>245</v>
       </c>
@@ -5621,7 +5614,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>93</v>
@@ -5633,7 +5626,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>246</v>
       </c>
@@ -5647,7 +5640,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>93</v>
@@ -5660,7 +5653,7 @@
       </c>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>247</v>
       </c>
@@ -5674,7 +5667,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>93</v>
@@ -5686,7 +5679,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>219</v>
       </c>
@@ -5704,7 +5697,7 @@
         <v>0.01</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>93</v>
@@ -5719,7 +5712,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>248</v>
       </c>
@@ -5733,7 +5726,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>93</v>
@@ -5748,7 +5741,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -5771,7 +5764,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>413</v>
       </c>
@@ -5782,7 +5775,7 @@
         <v>-1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J23" t="s">
         <v>205</v>
@@ -5794,7 +5787,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>414</v>
       </c>
@@ -5805,7 +5798,7 @@
         <v>-1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J24" t="s">
         <v>196</v>
@@ -5817,7 +5810,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>409</v>
       </c>
@@ -5825,7 +5818,7 @@
         <v>422</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J25" t="s">
         <v>277</v>
@@ -5834,7 +5827,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>410</v>
       </c>
@@ -5842,7 +5835,7 @@
         <v>424</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J26" t="s">
         <v>413</v>
@@ -5851,7 +5844,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>412</v>
       </c>
@@ -5862,7 +5855,7 @@
         <v>-1</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="J27" t="s">
         <v>409</v>
@@ -5871,7 +5864,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>417</v>
       </c>
@@ -5885,7 +5878,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>93</v>
@@ -5897,7 +5890,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>415</v>
       </c>
@@ -5908,7 +5901,7 @@
         <v>348</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>93</v>
@@ -5920,7 +5913,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>416</v>
       </c>
@@ -5934,7 +5927,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>93</v>
@@ -5946,7 +5939,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>461</v>
       </c>
@@ -5960,18 +5953,21 @@
         <v>3</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="J31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B32" t="s">
-        <v>465</v>
+        <v>546</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>347</v>
@@ -5980,15 +5976,24 @@
         <v>7</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" t="s">
+        <v>87</v>
+      </c>
+      <c r="J32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="B33" t="s">
-        <v>466</v>
+        <v>547</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>347</v>
@@ -5997,15 +6002,24 @@
         <v>8</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B34" t="s">
-        <v>467</v>
+        <v>548</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>347</v>
@@ -6014,15 +6028,24 @@
         <v>9</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I34" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="B35" t="s">
-        <v>468</v>
+        <v>549</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>347</v>
@@ -6031,15 +6054,24 @@
         <v>10</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" t="s">
+        <v>87</v>
+      </c>
+      <c r="J35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B36" t="s">
-        <v>469</v>
+        <v>550</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>347</v>
@@ -6048,15 +6080,24 @@
         <v>11</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I36" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>473</v>
+      </c>
+      <c r="B37" t="s">
         <v>551</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>479</v>
-      </c>
-      <c r="B37" t="s">
-        <v>470</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>347</v>
@@ -6065,15 +6106,24 @@
         <v>12</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I37" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>463</v>
       </c>
       <c r="B38" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>347</v>
@@ -6082,21 +6132,24 @@
         <v>4</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
+      </c>
+      <c r="I38" t="s">
+        <v>87</v>
       </c>
       <c r="J38" t="s">
-        <v>474</v>
+        <v>212</v>
       </c>
       <c r="K38" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>462</v>
       </c>
       <c r="B39" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>347</v>
@@ -6105,21 +6158,24 @@
         <v>5</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
+      </c>
+      <c r="I39" t="s">
+        <v>87</v>
       </c>
       <c r="J39" t="s">
-        <v>475</v>
+        <v>213</v>
       </c>
       <c r="K39" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>464</v>
       </c>
       <c r="B40" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>347</v>
@@ -6128,54 +6184,72 @@
         <v>6</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
+      </c>
+      <c r="I40" t="s">
+        <v>87</v>
       </c>
       <c r="J40" t="s">
+        <v>214</v>
+      </c>
+      <c r="K40" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>478</v>
+      </c>
+      <c r="B41" t="s">
+        <v>475</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="J41" t="s">
+        <v>277</v>
+      </c>
+      <c r="K41" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>479</v>
+      </c>
+      <c r="B42" t="s">
         <v>476</v>
       </c>
-      <c r="K40" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>484</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="F42" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="J42" t="s">
+        <v>276</v>
+      </c>
+      <c r="K42" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>480</v>
+      </c>
+      <c r="B43" t="s">
+        <v>477</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="J43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>481</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>485</v>
-      </c>
-      <c r="B42" t="s">
-        <v>482</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>486</v>
-      </c>
-      <c r="B43" t="s">
-        <v>483</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>487</v>
-      </c>
       <c r="B44" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>346</v>
@@ -6184,15 +6258,21 @@
         <v>3</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="H44" t="s">
+        <v>195</v>
+      </c>
+      <c r="J44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B45" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>346</v>
@@ -6201,15 +6281,21 @@
         <v>4</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="H45" t="s">
+        <v>198</v>
+      </c>
+      <c r="J45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B46" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>346</v>
@@ -6218,15 +6304,21 @@
         <v>5</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="H46" t="s">
+        <v>201</v>
+      </c>
+      <c r="J46" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B47" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>346</v>
@@ -6235,15 +6327,21 @@
         <v>7</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="H47" t="s">
+        <v>204</v>
+      </c>
+      <c r="J47" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B48" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>346</v>
@@ -6252,15 +6350,21 @@
         <v>8</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="H48" t="s">
+        <v>207</v>
+      </c>
+      <c r="J48" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="B49" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>346</v>
@@ -6269,15 +6373,21 @@
         <v>9</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="H49" t="s">
+        <v>210</v>
+      </c>
+      <c r="J49" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B50" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>346</v>
@@ -6286,15 +6396,24 @@
         <v>2</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="J50" t="s">
+        <v>195</v>
+      </c>
+      <c r="K50" t="s">
+        <v>198</v>
+      </c>
+      <c r="L50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B51" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>346</v>
@@ -6303,15 +6422,24 @@
         <v>6</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+      <c r="J51" t="s">
+        <v>204</v>
+      </c>
+      <c r="K51" t="s">
+        <v>207</v>
+      </c>
+      <c r="L51" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B52" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>346</v>
@@ -6320,16 +6448,17 @@
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
+      </c>
+      <c r="J52" t="s">
+        <v>488</v>
+      </c>
+      <c r="K52" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6337,24 +6466,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="75" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="118.109375" style="23" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="118.1640625" style="23" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
     <col min="9" max="9" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6380,10 +6509,10 @@
         <v>363</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>343</v>
       </c>
@@ -6406,7 +6535,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -6429,7 +6558,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>358</v>
       </c>
@@ -6450,10 +6579,10 @@
         <v>365</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A5" s="56" t="s">
         <v>405</v>
       </c>
@@ -6472,10 +6601,10 @@
         <v>445</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
         <v>406</v>
       </c>
@@ -6494,10 +6623,10 @@
         <v>446</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>366</v>
       </c>
@@ -6515,10 +6644,10 @@
         <v>401</v>
       </c>
       <c r="I7" s="41" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>367</v>
       </c>
@@ -6536,10 +6665,10 @@
         <v>402</v>
       </c>
       <c r="I8" s="53" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>368</v>
       </c>
@@ -6557,10 +6686,10 @@
         <v>403</v>
       </c>
       <c r="I9" s="54" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>392</v>
       </c>
@@ -6578,10 +6707,10 @@
         <v>394</v>
       </c>
       <c r="I10" s="52" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>372</v>
       </c>
@@ -6599,10 +6728,10 @@
         <v>395</v>
       </c>
       <c r="I11" s="55" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>375</v>
       </c>
@@ -6620,10 +6749,10 @@
         <v>447</v>
       </c>
       <c r="I12" s="52" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>396</v>
       </c>
@@ -6642,10 +6771,10 @@
         <v>377</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>397</v>
       </c>
@@ -6666,10 +6795,10 @@
         <v>379</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>398</v>
       </c>
@@ -6690,10 +6819,10 @@
         <v>380</v>
       </c>
       <c r="I15" s="53" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>381</v>
       </c>
@@ -6714,10 +6843,10 @@
         <v>393</v>
       </c>
       <c r="I16" s="53" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>220</v>
       </c>
@@ -6730,10 +6859,10 @@
         <v>425</v>
       </c>
       <c r="H17" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>221</v>
       </c>
@@ -6746,10 +6875,10 @@
         <v>425</v>
       </c>
       <c r="H18" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -6762,10 +6891,10 @@
         <v>425</v>
       </c>
       <c r="H19" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>249</v>
       </c>
@@ -6778,10 +6907,10 @@
         <v>425</v>
       </c>
       <c r="H20" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>250</v>
       </c>
@@ -6794,10 +6923,10 @@
         <v>425</v>
       </c>
       <c r="H21" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>251</v>
       </c>
@@ -6810,10 +6939,10 @@
         <v>425</v>
       </c>
       <c r="H22" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>360</v>
       </c>
@@ -6828,7 +6957,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -6846,7 +6975,7 @@
       </c>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -6863,7 +6992,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -6880,7 +7009,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -6897,7 +7026,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>291</v>
       </c>
@@ -6915,7 +7044,7 @@
       </c>
       <c r="H28" s="23"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>301</v>
       </c>
@@ -6932,7 +7061,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>302</v>
       </c>
@@ -6949,7 +7078,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>303</v>
       </c>
@@ -6966,7 +7095,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>294</v>
       </c>
@@ -6983,7 +7112,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -7000,7 +7129,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>305</v>
       </c>
@@ -7017,7 +7146,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>306</v>
       </c>
@@ -7034,7 +7163,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>314</v>
       </c>
@@ -7052,7 +7181,7 @@
       </c>
       <c r="H36" s="23"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>315</v>
       </c>
@@ -7069,7 +7198,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>290</v>
       </c>
@@ -7086,7 +7215,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>292</v>
       </c>
@@ -7103,7 +7232,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>293</v>
       </c>
@@ -7120,7 +7249,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>295</v>
       </c>
@@ -7137,7 +7266,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>223</v>
       </c>
@@ -7154,7 +7283,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>252</v>
       </c>
@@ -7171,7 +7300,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -7188,7 +7317,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>225</v>
       </c>
@@ -7205,7 +7334,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>226</v>
       </c>
@@ -7222,7 +7351,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>227</v>
       </c>
@@ -7242,10 +7371,10 @@
         <v>385</v>
       </c>
       <c r="I47" s="40" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>228</v>
       </c>
@@ -7265,10 +7394,10 @@
         <v>386</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>229</v>
       </c>
@@ -7288,10 +7417,10 @@
         <v>387</v>
       </c>
       <c r="I49" s="40" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>230</v>
       </c>
@@ -7311,10 +7440,10 @@
         <v>388</v>
       </c>
       <c r="I50" s="40" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>231</v>
       </c>
@@ -7335,7 +7464,7 @@
       </c>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>232</v>
       </c>
@@ -7355,10 +7484,10 @@
         <v>385</v>
       </c>
       <c r="I52" s="40" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>233</v>
       </c>
@@ -7378,10 +7507,10 @@
         <v>386</v>
       </c>
       <c r="I53" s="40" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>234</v>
       </c>
@@ -7401,10 +7530,10 @@
         <v>387</v>
       </c>
       <c r="I54" s="40" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>235</v>
       </c>
@@ -7424,10 +7553,10 @@
         <v>388</v>
       </c>
       <c r="I55" s="40" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>236</v>
       </c>
@@ -7448,7 +7577,7 @@
       </c>
       <c r="I56" s="23"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>237</v>
       </c>
@@ -7469,10 +7598,10 @@
         <v>385</v>
       </c>
       <c r="I57" s="40" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>238</v>
       </c>
@@ -7492,10 +7621,10 @@
         <v>386</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>239</v>
       </c>
@@ -7515,10 +7644,10 @@
         <v>387</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>240</v>
       </c>
@@ -7538,10 +7667,10 @@
         <v>388</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>453</v>
       </c>
@@ -7549,7 +7678,7 @@
         <v>67</v>
       </c>
       <c r="C61" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="D61" s="49">
         <v>0.06</v>
@@ -7558,10 +7687,10 @@
         <v>362</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>454</v>
       </c>
@@ -7569,7 +7698,7 @@
         <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="D62" s="49">
         <v>0.11</v>
@@ -7579,10 +7708,10 @@
         <v>362</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>455</v>
       </c>
@@ -7590,7 +7719,7 @@
         <v>449</v>
       </c>
       <c r="C63" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D63" s="49">
         <v>0.11</v>
@@ -7599,27 +7728,27 @@
         <v>362</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="C64" s="56" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="D64" s="50">
         <v>0.7</v>
       </c>
       <c r="I64" s="48" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>254</v>
       </c>
@@ -7634,7 +7763,7 @@
       </c>
       <c r="I65" s="23"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>255</v>
       </c>
@@ -7649,7 +7778,7 @@
       </c>
       <c r="I66" s="23"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>256</v>
       </c>
@@ -7664,7 +7793,7 @@
       </c>
       <c r="I67" s="23"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>257</v>
       </c>
@@ -7684,10 +7813,10 @@
         <v>385</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>258</v>
       </c>
@@ -7707,10 +7836,10 @@
         <v>386</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>259</v>
       </c>
@@ -7730,10 +7859,10 @@
         <v>387</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>260</v>
       </c>
@@ -7754,7 +7883,7 @@
       </c>
       <c r="I71" s="23"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>261</v>
       </c>
@@ -7775,7 +7904,7 @@
       </c>
       <c r="I72" s="23"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>263</v>
       </c>
@@ -7795,10 +7924,10 @@
         <v>385</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>264</v>
       </c>
@@ -7818,10 +7947,10 @@
         <v>386</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>265</v>
       </c>
@@ -7841,10 +7970,10 @@
         <v>387</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>266</v>
       </c>
@@ -7865,7 +7994,7 @@
       </c>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>267</v>
       </c>
@@ -7886,7 +8015,7 @@
       </c>
       <c r="I77" s="23"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>268</v>
       </c>
@@ -7906,10 +8035,10 @@
         <v>385</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>269</v>
       </c>
@@ -7929,10 +8058,10 @@
         <v>386</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>270</v>
       </c>
@@ -7952,10 +8081,10 @@
         <v>387</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>271</v>
       </c>
@@ -7975,18 +8104,18 @@
         <v>388</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C82" s="56" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="D82" s="49">
         <v>0.2</v>
@@ -7995,10 +8124,10 @@
         <v>362</v>
       </c>
       <c r="I82" s="48" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>456</v>
       </c>
@@ -8016,7 +8145,7 @@
       </c>
       <c r="I83" s="23"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>457</v>
       </c>
@@ -8024,16 +8153,16 @@
         <v>452</v>
       </c>
       <c r="C84" s="56" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="D84" s="49">
         <v>0.11</v>
       </c>
       <c r="I84" s="45" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>458</v>
       </c>
@@ -8041,16 +8170,16 @@
         <v>451</v>
       </c>
       <c r="C85" s="56" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="D85" s="49">
         <v>0.11</v>
       </c>
       <c r="I85" s="45" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -8072,7 +8201,7 @@
       </c>
       <c r="I86" s="23"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>436</v>
       </c>
@@ -8093,7 +8222,7 @@
       </c>
       <c r="I87" s="44"/>
     </row>
-    <row r="88" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>433</v>
       </c>
@@ -8113,10 +8242,10 @@
         <v>431</v>
       </c>
       <c r="I88" s="59" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>434</v>
       </c>
@@ -8137,10 +8266,10 @@
         <v>431</v>
       </c>
       <c r="I89" s="60" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>435</v>
       </c>
@@ -8160,10 +8289,10 @@
         <v>431</v>
       </c>
       <c r="I90" s="58" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>438</v>
       </c>
@@ -8183,10 +8312,10 @@
         <v>431</v>
       </c>
       <c r="I91" s="58" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>437</v>
       </c>
@@ -8207,22 +8336,17 @@
       </c>
       <c r="I92" s="61"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I93" s="62" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I94" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8234,13 +8358,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>135</v>
       </c>
@@ -8248,7 +8372,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -8256,7 +8380,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>346</v>
       </c>
@@ -8264,15 +8388,15 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>138</v>
       </c>
@@ -8280,7 +8404,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>347</v>
       </c>
@@ -8288,7 +8412,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>140</v>
       </c>
@@ -8296,23 +8420,23 @@
         <v>426</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>348</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>459</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>425</v>
       </c>
@@ -8322,10 +8446,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>